<commit_message>
DataAnalysis Data index system (To be continued)
</commit_message>
<xml_diff>
--- a/Py_DataScience/Theory_Note/数据指标体系/11.4数据指标体系.xlsx
+++ b/Py_DataScience/Theory_Note/数据指标体系/11.4数据指标体系.xlsx
@@ -1,24 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ztnn/data-analysis/11-数据指标体系/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xu\Desktop\PythonDevelopment\DataAnalysis\Py_DataScience\Theory_Note\数据指标体系\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6ADCB89-068B-ED40-96F7-B535B381688C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66338387-0385-4F71-8C02-83C131E22AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="460" windowWidth="24760" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="分析指标1.0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -108,39 +118,21 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>下载量</t>
-  </si>
-  <si>
     <t>安装量</t>
   </si>
   <si>
-    <t>设备激活量</t>
-  </si>
-  <si>
-    <t>新手教程完成量</t>
-  </si>
-  <si>
     <t>距离上次登录的时间</t>
   </si>
   <si>
-    <t>流失率</t>
-  </si>
-  <si>
     <t>次日留存率</t>
   </si>
   <si>
     <t>3日留存率</t>
   </si>
   <si>
-    <t>7日留存率</t>
-  </si>
-  <si>
     <t>30日留存率</t>
   </si>
   <si>
-    <t>每日流失量</t>
-  </si>
-  <si>
     <t>案例分析</t>
     <rPh sb="0" eb="1">
       <t>an'li</t>
@@ -157,38 +149,6 @@
     <t>分享次数</t>
   </si>
   <si>
-    <t>UV 独立访客数</t>
-    <rPh sb="3" eb="4">
-      <t>du'li'fang'ke'shu</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PV 页面浏览量/点击数</t>
-    <rPh sb="3" eb="4">
-      <t>ye'mian</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>liu'lan'liang</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>dian'ji'shu</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DNU 日新增用户数</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CVR 渠道转化率</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CAC 用户获取成本</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>WAU 周活跃用户数</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -202,16 +162,6 @@
   </si>
   <si>
     <t>DAU 日活跃用户数</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DAU / MAU 用户黏性</t>
-    <rPh sb="10" eb="11">
-      <t>yong'hu</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>nian'xign</t>
-    </rPh>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -266,16 +216,6 @@
     </rPh>
     <rPh sb="3" eb="4">
       <t>kou'bei'qu'dao</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>病毒系数K</t>
-    <rPh sb="0" eb="1">
-      <t>bing'du</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>xi'shu</t>
     </rPh>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -628,10 +568,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>曝光量</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>AARRR</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -761,9 +697,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>分享回流比</t>
-  </si>
-  <si>
     <t>广告变现</t>
     <rPh sb="0" eb="1">
       <t>guang'gao</t>
@@ -813,16 +746,6 @@
     </rPh>
     <rPh sb="2" eb="3">
       <t>bian'xian</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PUR 付费渗透率</t>
-    <rPh sb="4" eb="5">
-      <t>fu'fei</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>shen'tou'lv</t>
     </rPh>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -938,18 +861,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ARPU 平均每用户收入(Average Revenue Per User)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ARPPU 平均每付费用户收入Average Revenue Per Paying User)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LTV 用户生命周期价值</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>病毒传播</t>
     <rPh sb="0" eb="1">
       <t>bing'du</t>
@@ -970,49 +881,88 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>订单数</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>参与</t>
+    <rPh sb="0" eb="1">
+      <t>can'yu</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>曝光量 (被多少人看到了)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">下载量 </t>
+  </si>
+  <si>
+    <t>PV 页面浏览量/点击数 (PagevView)</t>
+  </si>
+  <si>
+    <t>UV 独立访客数 (有多少用户看了) Unique Visitor</t>
+  </si>
+  <si>
+    <t>DNU 日新增用户数 (Day New User)</t>
+  </si>
+  <si>
+    <t>CVR 渠道转化率 (Conversion Rate) 每个平台注册/每个平台点击</t>
+  </si>
+  <si>
+    <t>CAC 用户获取成本 (Customer Acquisition Cost) 营销费用/获客数量</t>
+  </si>
+  <si>
+    <t>设备激活量 (点开app次数)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新手教程完成量 </t>
+  </si>
+  <si>
+    <t>DAU / MAU 用户黏性 (高频 0.5)</t>
+  </si>
+  <si>
+    <t>每日流失量 (日活的差值)</t>
+  </si>
+  <si>
+    <t>流失率 (流失用户/总用户数)</t>
+  </si>
+  <si>
+    <t>7日留存率 (活跃用户/同批新增用户)</t>
+  </si>
+  <si>
+    <t>分享回流比 (跳回量/分享量)</t>
+  </si>
+  <si>
+    <t>GMV 总成交额 (Gross Merchandise Volume)</t>
+  </si>
+  <si>
+    <t>PUR 付费渗透率 (付费用户/活跃用户)</t>
+  </si>
+  <si>
     <t>付费频次</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PCT 客单价/平均购买金额</t>
-    <rPh sb="8" eb="9">
-      <t>ping'jun</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>gou'mai</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>jin'e</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>订单数</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GMV 总成交额</t>
-    <rPh sb="4" eb="5">
-      <t>zong</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>cheng'jiao'e</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>参与</t>
-    <rPh sb="0" eb="1">
-      <t>can'yu</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCT 客单价/平均购买金额 (消费总额/频次)</t>
+  </si>
+  <si>
+    <t>ARPU 平均每用户收入(Average Revenue Per User) 总收入/活跃用户</t>
+  </si>
+  <si>
+    <t>ARPPU 平均每付费用户收入Average Revenue Per Paying User) 总收入/付费用户</t>
+  </si>
+  <si>
+    <t>LTV 用户生命周期价值 LT [平均生命周期 7天走 14天走 21天走] * ARPU  (体现企业有多赚钱)</t>
+  </si>
+  <si>
+    <t>病毒系数K (付费流量对自然流量的影响程度)  转发分享带来的用户量</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1381,13 +1331,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1424,8 +1374,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>240169</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>183248</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>352581</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1963,20 +1913,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="133" zoomScaleNormal="255" zoomScalePageLayoutView="255" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="255" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.81640625" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
-    <col min="2" max="6" width="25.33203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="14.83203125" style="1"/>
+    <col min="1" max="1" width="13.6328125" style="2" customWidth="1"/>
+    <col min="2" max="6" width="25.36328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="31.05" customHeight="1" thickBot="1">
       <c r="A1" s="27" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -1984,9 +1934,9 @@
       <c r="E1" s="28"/>
       <c r="F1" s="29"/>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="3" customFormat="1">
       <c r="A2" s="30" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -2004,7 +1954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="16.2" thickBot="1">
       <c r="A3" s="31"/>
       <c r="B3" s="11" t="s">
         <v>5</v>
@@ -2019,18 +1969,18 @@
         <v>10</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.2" thickBot="1">
       <c r="A4" s="15" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>9</v>
@@ -2042,385 +1992,385 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="33" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="33"/>
       <c r="B6" s="4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.2" thickBot="1">
       <c r="A7" s="37"/>
       <c r="B7" s="7" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="33" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="33"/>
       <c r="B9" s="4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="33"/>
       <c r="B10" s="4" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="33"/>
       <c r="B11" s="4" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.2" thickBot="1">
       <c r="A12" s="33"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="16.2" thickBot="1">
+      <c r="A13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="31.8" thickBot="1">
+      <c r="A14" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="46.8">
+      <c r="A15" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="F15" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="31.2">
       <c r="A16" s="32"/>
       <c r="B16" s="4" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>23</v>
+        <v>106</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="31.2">
       <c r="A17" s="32"/>
       <c r="B17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="31.2">
       <c r="A18" s="32"/>
       <c r="B18" s="4" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="46.8">
       <c r="A19" s="32"/>
       <c r="B19" s="4" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="31.2">
       <c r="A20" s="32"/>
       <c r="B20" s="4" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>21</v>
+        <v>108</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="F20" s="26"/>
     </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="46.8">
       <c r="A21" s="32"/>
       <c r="B21" s="4" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="F21" s="26"/>
     </row>
-    <row r="22" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="63" thickBot="1">
       <c r="A22" s="32"/>
       <c r="B22" s="4" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="34" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="35"/>
       <c r="B24" s="4" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="16.2" thickBot="1">
       <c r="A25" s="36"/>
       <c r="B25" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:6" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="90" customHeight="1" thickBot="1">
       <c r="A26" s="18" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="22"/>

</xml_diff>